<commit_message>
FullStack Developer 1st commit
</commit_message>
<xml_diff>
--- a/Practical WEBDEV Learning/Practise/JS Assignment/Practice Sheet_JavaScript.xlsx
+++ b/Practical WEBDEV Learning/Practise/JS Assignment/Practice Sheet_JavaScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Firey Beast\Desktop\Web Development\Practical WEBDEV Learning\Practise\JS Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C405E4-A6A8-4AD4-9447-A472A8C84D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BF6CD-5C95-436B-8CC0-3DDFD277BC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Practical Javscript Practice Sheet</t>
   </si>
@@ -758,7 +758,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -832,7 +832,9 @@
       <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="33" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -844,7 +846,9 @@
       <c r="C6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="33" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -856,7 +860,9 @@
       <c r="C7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="33" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">

</xml_diff>